<commit_message>
Added convert names fcn
</commit_message>
<xml_diff>
--- a/draft.xlsx
+++ b/draft.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomo/Postdoc_BMI_UWO/python/games-played/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B21FD8-DA74-F74C-8F00-6658F2882AFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="15160" windowHeight="17220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FantraxDraftResults_Honolulu Le" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -57,9 +63,6 @@
     <t>PHI</t>
   </si>
   <si>
-    <t>Derrick Rossi</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:03:28</t>
   </si>
   <si>
@@ -75,9 +78,6 @@
     <t>POR</t>
   </si>
   <si>
-    <t>Follow Leite</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:06:21</t>
   </si>
   <si>
@@ -90,9 +90,6 @@
     <t>DEN</t>
   </si>
   <si>
-    <t>Civezzano Maned Meerkats</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:08:22</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>MIL</t>
   </si>
   <si>
-    <t>MISSION #1</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:10:21</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>ORL</t>
   </si>
   <si>
-    <t>Masonville Graveyard</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:12:42</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>NY</t>
   </si>
   <si>
-    <t>Borgo Ciodo Hammers</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:14:09</t>
   </si>
   <si>
@@ -231,9 +219,6 @@
     <t>MIN</t>
   </si>
   <si>
-    <t>Inglewood Lightnings</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:24:56</t>
   </si>
   <si>
@@ -246,9 +231,6 @@
     <t>GS</t>
   </si>
   <si>
-    <t>Steel Panthers</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:40:36</t>
   </si>
   <si>
@@ -309,9 +291,6 @@
     <t>Bam Adebayo</t>
   </si>
   <si>
-    <t>Golden Goffers</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:52:00</t>
   </si>
   <si>
@@ -324,9 +303,6 @@
     <t>IND</t>
   </si>
   <si>
-    <t>Artists of Life</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 8:53:49</t>
   </si>
   <si>
@@ -366,9 +342,6 @@
     <t>PHO</t>
   </si>
   <si>
-    <t>Arbizzano Owls</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 9:01:11</t>
   </si>
   <si>
@@ -477,9 +450,6 @@
     <t>OKC</t>
   </si>
   <si>
-    <t>LA Samras</t>
-  </si>
-  <si>
     <t>Oct 17, 2021 9:19:12</t>
   </si>
   <si>
@@ -1372,12 +1342,48 @@
   </si>
   <si>
     <t>Oct 17, 2021 11:40:09</t>
+  </si>
+  <si>
+    <t>DER</t>
+  </si>
+  <si>
+    <t>FWL</t>
+  </si>
+  <si>
+    <t>CVZ</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>MVB</t>
+  </si>
+  <si>
+    <t>BCH</t>
+  </si>
+  <si>
+    <t>IGWL</t>
+  </si>
+  <si>
+    <t>STLP</t>
+  </si>
+  <si>
+    <t>GOF</t>
+  </si>
+  <si>
+    <t>PIMA</t>
+  </si>
+  <si>
+    <t>LIFE</t>
+  </si>
+  <si>
+    <t>SAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1415,6 +1421,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1739,16 +1753,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A133"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1774,7 +1788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1794,41 +1808,41 @@
         <v>55</v>
       </c>
       <c r="G2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>14</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
       <c r="F3">
         <v>60</v>
       </c>
       <c r="G3" t="s">
+        <v>440</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>20</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1837,76 +1851,76 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5">
         <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1915,180 +1929,180 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F7">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F9">
         <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F10">
         <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>69</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F13">
         <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2097,180 +2111,180 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F14">
         <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F15">
         <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F16">
         <v>61</v>
       </c>
       <c r="G16" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F17">
         <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F18">
         <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F19">
         <v>56</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F20">
         <v>45</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -2279,232 +2293,232 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F21">
         <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F22">
         <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F23">
         <v>22</v>
       </c>
       <c r="G23" t="s">
+        <v>447</v>
+      </c>
+      <c r="H23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>96</v>
-      </c>
-      <c r="H23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>106</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F25">
         <v>29</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E26" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F26">
         <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F27">
         <v>18</v>
       </c>
       <c r="G27" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F28">
         <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E29" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F29">
         <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -2513,24 +2527,24 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E30" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F30">
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -2539,111 +2553,111 @@
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E31" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F31">
         <v>29</v>
       </c>
       <c r="G31" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F32">
         <v>39</v>
       </c>
       <c r="G32" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F33">
         <v>30</v>
       </c>
       <c r="G33" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E34" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F34">
         <v>19</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
@@ -2652,336 +2666,336 @@
         <v>20</v>
       </c>
       <c r="G35" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H35" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E36" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F36">
         <v>25</v>
       </c>
       <c r="G36" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H36" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="E37" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F37">
         <v>18</v>
       </c>
       <c r="G37" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H37" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F38">
         <v>24</v>
       </c>
       <c r="G38" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F39">
         <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F40">
         <v>38</v>
       </c>
       <c r="G40" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H40" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F41">
         <v>39</v>
       </c>
       <c r="G41" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H41" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" t="s">
         <v>46</v>
-      </c>
-      <c r="D42" t="s">
-        <v>172</v>
-      </c>
-      <c r="E42" t="s">
-        <v>52</v>
       </c>
       <c r="F42">
         <v>27</v>
       </c>
       <c r="G42" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H42" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E43" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F43">
         <v>20</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H43" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E44" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F44">
         <v>20</v>
       </c>
       <c r="G44" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H44" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D45" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E45" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F45">
         <v>27</v>
       </c>
       <c r="G45" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E46" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F46">
         <v>29</v>
       </c>
       <c r="G46" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H46" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E47" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F47">
         <v>49</v>
       </c>
       <c r="G47" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H47" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E48" t="s">
         <v>11</v>
@@ -2990,41 +3004,41 @@
         <v>19</v>
       </c>
       <c r="G48" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H48" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="E49" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F49">
         <v>26</v>
       </c>
       <c r="G49" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H49" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B50">
         <v>49</v>
@@ -3033,24 +3047,24 @@
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="E50" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F50">
         <v>23</v>
       </c>
       <c r="G50" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H50" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B51">
         <v>50</v>
@@ -3059,50 +3073,50 @@
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E51" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F51">
         <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H51" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D52" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="E52" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F52">
         <v>9</v>
       </c>
       <c r="G52" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H52" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="B53">
         <v>52</v>
@@ -3111,24 +3125,24 @@
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F53">
         <v>33</v>
       </c>
       <c r="G53" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H53" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B54">
         <v>53</v>
@@ -3137,76 +3151,76 @@
         <v>9</v>
       </c>
       <c r="D54" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F54">
         <v>20</v>
       </c>
       <c r="G54" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H54" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B55">
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D55" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F55">
         <v>18</v>
       </c>
       <c r="G55" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H55" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B56">
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D56" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E56" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F56">
         <v>7</v>
       </c>
       <c r="G56" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H56" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="B57">
         <v>56</v>
@@ -3215,232 +3229,232 @@
         <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="E57" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F57">
         <v>15</v>
       </c>
       <c r="G57" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H57" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D58" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E58" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F58">
         <v>24</v>
       </c>
       <c r="G58" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H58" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B59">
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="E59" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F59">
         <v>15</v>
       </c>
       <c r="G59" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H59" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D60" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F60">
         <v>8</v>
       </c>
       <c r="G60" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H60" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="E61" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F61">
         <v>11</v>
       </c>
       <c r="G61" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H61" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="E62" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F62">
         <v>12</v>
       </c>
       <c r="G62" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H62" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D63" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="E63" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F63">
         <v>18</v>
       </c>
       <c r="G63" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H63" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D64" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="E64" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F64">
         <v>24</v>
       </c>
       <c r="G64" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H64" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B65">
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D65" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="E65" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F65">
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H65" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B66">
         <v>65</v>
@@ -3449,24 +3463,24 @@
         <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="E66" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F66">
         <v>6</v>
       </c>
       <c r="G66" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H66" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B67">
         <v>66</v>
@@ -3475,50 +3489,50 @@
         <v>9</v>
       </c>
       <c r="D67" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="E67" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F67">
         <v>16</v>
       </c>
       <c r="G67" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H67" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B68">
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="E68" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F68">
         <v>7</v>
       </c>
       <c r="G68" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H68" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B69">
         <v>68</v>
@@ -3527,284 +3541,284 @@
         <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="E69" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F69">
         <v>5</v>
       </c>
       <c r="G69" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H69" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D70" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="E70" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F70">
         <v>6</v>
       </c>
       <c r="G70" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H70" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D71" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="E71" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F71">
         <v>9</v>
       </c>
       <c r="G71" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H71" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B72">
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="E72" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F72">
         <v>6</v>
       </c>
       <c r="G72" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H72" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="B73">
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E73" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F73">
         <v>28</v>
       </c>
       <c r="G73" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H73" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D74" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="E74" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F74">
         <v>16</v>
       </c>
       <c r="G74" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H74" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B75">
         <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D75" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="E75" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="F75">
         <v>8</v>
       </c>
       <c r="G75" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H75" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B76">
         <v>75</v>
       </c>
       <c r="C76" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D76" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E76" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F76">
         <v>19</v>
       </c>
       <c r="G76" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H76" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="B77">
         <v>76</v>
       </c>
       <c r="C77" t="s">
+        <v>53</v>
+      </c>
+      <c r="D77" t="s">
+        <v>269</v>
+      </c>
+      <c r="E77" t="s">
         <v>59</v>
-      </c>
-      <c r="D77" t="s">
-        <v>281</v>
-      </c>
-      <c r="E77" t="s">
-        <v>65</v>
       </c>
       <c r="F77">
         <v>1</v>
       </c>
       <c r="G77" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H77" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B78">
         <v>77</v>
       </c>
       <c r="C78" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="E78" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="F78">
         <v>30</v>
       </c>
       <c r="G78" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H78" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="B79">
         <v>78</v>
       </c>
       <c r="C79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="E79" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F79">
         <v>6</v>
       </c>
       <c r="G79" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H79" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -3813,102 +3827,102 @@
         <v>9</v>
       </c>
       <c r="D80" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E80" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="F80">
         <v>19</v>
       </c>
       <c r="G80" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H80" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="B81">
         <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D81" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="E81" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F81">
         <v>2</v>
       </c>
       <c r="G81" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H81" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="B82">
         <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="E82" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F82">
         <v>6</v>
       </c>
       <c r="G82" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H82" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B83">
         <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D83" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F83">
         <v>12</v>
       </c>
       <c r="G83" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H83" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -3917,50 +3931,50 @@
         <v>9</v>
       </c>
       <c r="D84" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="E84" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F84">
         <v>1</v>
       </c>
       <c r="G84" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H84" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="B85">
         <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D85" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="E85" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F85">
         <v>10</v>
       </c>
       <c r="G85" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H85" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -3969,102 +3983,102 @@
         <v>9</v>
       </c>
       <c r="D86" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="E86" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F86">
         <v>7</v>
       </c>
       <c r="G86" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H86" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B87">
         <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="E87" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F87">
         <v>3</v>
       </c>
       <c r="G87" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H87" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="B88">
         <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D88" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="E88" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F88">
         <v>6</v>
       </c>
       <c r="G88" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H88" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="B89">
         <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D89" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="E89" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F89">
         <v>3</v>
       </c>
       <c r="G89" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H89" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -4073,50 +4087,50 @@
         <v>9</v>
       </c>
       <c r="D90" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="E90" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F90">
         <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H90" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="B91">
         <v>90</v>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D91" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="E91" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F91">
         <v>1</v>
       </c>
       <c r="G91" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H91" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -4125,206 +4139,206 @@
         <v>9</v>
       </c>
       <c r="D92" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="E92" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F92">
         <v>4</v>
       </c>
       <c r="G92" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H92" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B93">
         <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="E93" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F93">
         <v>7</v>
       </c>
       <c r="G93" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H93" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B94">
         <v>93</v>
       </c>
       <c r="C94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="E94" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F94">
         <v>4</v>
       </c>
       <c r="G94" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H94" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="B95">
         <v>94</v>
       </c>
       <c r="C95" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D95" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="E95" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F95">
         <v>14</v>
       </c>
       <c r="G95" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H95" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="B96">
         <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D96" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="E96" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F96">
         <v>5</v>
       </c>
       <c r="G96" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H96" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="B97">
         <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D97" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="E97" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F97">
         <v>4</v>
       </c>
       <c r="G97" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H97" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="B98">
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D98" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="E98" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F98">
         <v>16</v>
       </c>
       <c r="G98" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H98" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="B99">
         <v>98</v>
       </c>
       <c r="C99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="E99" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F99">
         <v>15</v>
       </c>
       <c r="G99" t="s">
-        <v>152</v>
+        <v>450</v>
       </c>
       <c r="H99" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -4333,258 +4347,258 @@
         <v>9</v>
       </c>
       <c r="D100" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="E100" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F100">
         <v>6</v>
       </c>
       <c r="G100" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H100" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="B101">
         <v>100</v>
       </c>
       <c r="C101" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D101" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="E101" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F101">
         <v>1</v>
       </c>
       <c r="G101" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H101" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="B102">
         <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D102" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="E102" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F102">
         <v>5</v>
       </c>
       <c r="G102" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H102" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="B103">
         <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D103" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="E103" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F103">
         <v>9</v>
       </c>
       <c r="G103" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="H103" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="B104">
         <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D104" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="E104" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F104">
         <v>3</v>
       </c>
       <c r="G104" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H104" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="B105">
         <v>104</v>
       </c>
       <c r="C105" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="E105" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F105">
         <v>3</v>
       </c>
       <c r="G105" t="s">
-        <v>115</v>
+        <v>449</v>
       </c>
       <c r="H105" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="B106">
         <v>105</v>
       </c>
       <c r="C106" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D106" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="E106" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F106">
         <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H106" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="B107">
         <v>106</v>
       </c>
       <c r="C107" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D107" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="E107" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F107">
         <v>2</v>
       </c>
       <c r="G107" t="s">
-        <v>38</v>
+        <v>443</v>
       </c>
       <c r="H107" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="B108">
         <v>107</v>
       </c>
       <c r="C108" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D108" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="E108" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F108">
         <v>3</v>
       </c>
       <c r="G108" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H108" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="B109">
         <v>108</v>
       </c>
       <c r="C109" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D109" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="E109" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F109">
         <v>1</v>
       </c>
       <c r="G109" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H109" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="B110">
         <v>109</v>
@@ -4593,336 +4607,336 @@
         <v>9</v>
       </c>
       <c r="D110" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="E110" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F110">
         <v>1</v>
       </c>
       <c r="G110" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H110" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="B111">
         <v>110</v>
       </c>
       <c r="C111" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D111" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="E111" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F111">
         <v>1</v>
       </c>
       <c r="G111" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H111" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="B112">
         <v>111</v>
       </c>
       <c r="C112" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D112" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="E112" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F112">
         <v>2</v>
       </c>
       <c r="G112" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H112" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="B113">
         <v>112</v>
       </c>
       <c r="C113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="E113" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F113">
         <v>7</v>
       </c>
       <c r="G113" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H113" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="B114">
         <v>113</v>
       </c>
       <c r="C114" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D114" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="E114" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F114">
         <v>4</v>
       </c>
       <c r="G114" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H114" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="B115">
         <v>114</v>
       </c>
       <c r="C115" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="E115" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F115">
         <v>1</v>
       </c>
       <c r="G115" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H115" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="B116">
         <v>115</v>
       </c>
       <c r="C116" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D116" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="E116" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F116">
         <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H116" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="B117">
         <v>116</v>
       </c>
       <c r="C117" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D117" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="E117" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F117">
         <v>4</v>
       </c>
       <c r="G117" t="s">
-        <v>101</v>
+        <v>448</v>
       </c>
       <c r="H117" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="B118">
         <v>117</v>
       </c>
       <c r="C118" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D118" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="E118" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F118">
         <v>1</v>
       </c>
       <c r="G118" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H118" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="B119">
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D119" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="E119" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F119">
         <v>5</v>
       </c>
       <c r="G119" t="s">
-        <v>96</v>
+        <v>447</v>
       </c>
       <c r="H119" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="B120">
         <v>119</v>
       </c>
       <c r="C120" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D120" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="E120" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F120">
         <v>1</v>
       </c>
       <c r="G120" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H120" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B121">
         <v>120</v>
       </c>
       <c r="C121" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D121" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="E121" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="F121">
         <v>2</v>
       </c>
       <c r="G121" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H121" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="B122">
         <v>121</v>
       </c>
       <c r="C122" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D122" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="E122" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F122">
         <v>2</v>
       </c>
       <c r="G122" t="s">
-        <v>75</v>
+        <v>446</v>
       </c>
       <c r="H122" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="B123">
         <v>122</v>
@@ -4931,7 +4945,7 @@
         <v>9</v>
       </c>
       <c r="D123" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -4940,270 +4954,270 @@
         <v>1</v>
       </c>
       <c r="G123" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H123" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="B124">
         <v>123</v>
       </c>
       <c r="C124" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D124" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="E124" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F124">
         <v>2</v>
       </c>
       <c r="G124" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H124" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="B125">
         <v>124</v>
       </c>
       <c r="C125" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D125" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="E125" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F125">
         <v>1</v>
       </c>
       <c r="G125" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H125" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="B126">
         <v>125</v>
       </c>
       <c r="C126" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D126" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="E126" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F126">
         <v>1</v>
       </c>
       <c r="G126" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="H126" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B127">
         <v>126</v>
       </c>
       <c r="C127" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D127" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="E127" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F127">
         <v>1</v>
       </c>
       <c r="G127" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="H127" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="B128">
         <v>127</v>
       </c>
       <c r="C128" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D128" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="E128" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F128">
         <v>1</v>
       </c>
       <c r="G128" t="s">
-        <v>23</v>
+        <v>441</v>
       </c>
       <c r="H128" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B129">
         <v>128</v>
       </c>
       <c r="C129" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D129" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="E129" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F129">
         <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H129" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="B130">
         <v>129</v>
       </c>
       <c r="C130" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D130" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="E130" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F130">
         <v>6</v>
       </c>
       <c r="G130" t="s">
-        <v>43</v>
+        <v>444</v>
       </c>
       <c r="H130" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="B131">
         <v>130</v>
       </c>
       <c r="C131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D131" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="E131" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F131">
         <v>1</v>
       </c>
       <c r="G131" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H131" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="B132">
         <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D132" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="E132" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F132">
         <v>1</v>
       </c>
       <c r="G132" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H132" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="B133">
         <v>132</v>
       </c>
       <c r="C133" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D133" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="E133" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F133">
         <v>1</v>
       </c>
       <c r="G133" t="s">
-        <v>18</v>
+        <v>440</v>
       </c>
       <c r="H133" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>